<commit_message>
Modify sample data file in test.xlsx
</commit_message>
<xml_diff>
--- a/src/sample_data/test.xlsx
+++ b/src/sample_data/test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GDP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GDP\src\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7515"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7515" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -21,23 +21,234 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Hello World !</t>
-  </si>
-  <si>
-    <t>data in sheet 1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
+  <si>
+    <t>S.No</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>X6</t>
+  </si>
+  <si>
+    <t>X7</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Z1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>Z2</t>
+  </si>
+  <si>
+    <t>Y3</t>
+  </si>
+  <si>
+    <t>Z3</t>
+  </si>
+  <si>
+    <t>Y4</t>
+  </si>
+  <si>
+    <t>Z4</t>
+  </si>
+  <si>
+    <t>Y5</t>
+  </si>
+  <si>
+    <t>Z5</t>
+  </si>
+  <si>
+    <t>Y6</t>
+  </si>
+  <si>
+    <t>Z6</t>
+  </si>
+  <si>
+    <t>Y7</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>H7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,8 +271,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,38 +579,562 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2">
+        <v>11111111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6">
+        <v>55555555</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7">
+        <v>66666666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>77777777</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9">
+        <v>88888888</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10">
+        <v>99999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <v>111111110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <v>122222221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13">
+        <v>133333332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <v>144444443</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15">
+        <v>155555554</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16">
+        <v>166666665</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17">
+        <v>177777776</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18">
+        <v>188888887</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19">
+        <v>199999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20">
+        <v>211111109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21">
+        <v>222222220</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>